<commit_message>
Update excel w/ links
</commit_message>
<xml_diff>
--- a/excel/space.xlsx
+++ b/excel/space.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="solar system" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="planet type" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="planetary feature" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="satellite" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="large body object" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="small body object" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="space phenomena" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="constellation" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="solar system" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="planet type" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="planetary feature" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="satellite" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="large body object" sheetId="5" r:id="rId9"/>
+    <sheet state="visible" name="small body object" sheetId="6" r:id="rId10"/>
+    <sheet state="visible" name="space phenomena" sheetId="7" r:id="rId11"/>
+    <sheet state="visible" name="constellation" sheetId="8" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
   <si>
     <t>class</t>
   </si>
@@ -32,6 +32,9 @@
     <t>synonym</t>
   </si>
   <si>
+    <t>dbXref</t>
+  </si>
+  <si>
     <t>sol</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
     <t>star; the sun</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/sun/</t>
+  </si>
+  <si>
     <t>inner system</t>
   </si>
   <si>
@@ -59,12 +65,18 @@
     <t>the world</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/earth/</t>
+  </si>
+  <si>
     <t>mars</t>
   </si>
   <si>
     <t>red planet</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/mars/</t>
+  </si>
+  <si>
     <t>outer system</t>
   </si>
   <si>
@@ -143,12 +155,18 @@
     <t>hubble space telescope</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/mission/hubble/</t>
+  </si>
+  <si>
     <t>international space station</t>
   </si>
   <si>
     <t>ISS</t>
   </si>
   <si>
+    <t>https://www.nasa.gov/international-space-station/</t>
+  </si>
+  <si>
     <t>lunar reconnaissance orbiter</t>
   </si>
   <si>
@@ -170,6 +188,9 @@
     <t>the moon</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/moon/</t>
+  </si>
+  <si>
     <t>europa</t>
   </si>
   <si>
@@ -197,6 +218,9 @@
     <t>planetoid</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/solar-system/asteroids/</t>
+  </si>
+  <si>
     <t>meteoroid</t>
   </si>
   <si>
@@ -206,13 +230,22 @@
     <t>space rock</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/solar-system/meteors-meteorites/</t>
+  </si>
+  <si>
     <t>comet</t>
   </si>
   <si>
     <t>formed of ice and dust with tails</t>
   </si>
   <si>
+    <t>https://science.nasa.gov/solar-system/comets/</t>
+  </si>
+  <si>
     <t>black hole</t>
+  </si>
+  <si>
+    <t>https://science.nasa.gov/universe/black-holes/</t>
   </si>
   <si>
     <t>nebula</t>
@@ -300,7 +333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -311,6 +344,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -327,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -335,6 +372,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -373,6 +413,10 @@
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,104 +636,121 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId2" ref="E5"/>
+    <hyperlink r:id="rId3" ref="E6"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -713,34 +774,37 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -771,41 +835,44 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -840,83 +907,100 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E3"/>
+    <hyperlink r:id="rId2" ref="E4"/>
+    <hyperlink r:id="rId3" ref="E7"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -940,23 +1024,26 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -987,39 +1074,56 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D3"/>
+    <hyperlink r:id="rId3" ref="D4"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1046,41 +1150,54 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D5"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1107,141 +1224,144 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel with xrefs and external resources
</commit_message>
<xml_diff>
--- a/excel/space.xlsx
+++ b/excel/space.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="109">
   <si>
     <t>class</t>
   </si>
@@ -35,6 +35,9 @@
     <t>dbXref</t>
   </si>
   <si>
+    <t>externalResource</t>
+  </si>
+  <si>
     <t>sol</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
     <t>star; the sun</t>
   </si>
   <si>
+    <t>WD:Q525</t>
+  </si>
+  <si>
     <t>https://science.nasa.gov/sun/</t>
   </si>
   <si>
@@ -65,6 +71,9 @@
     <t>the world</t>
   </si>
   <si>
+    <t>WD:Q2</t>
+  </si>
+  <si>
     <t>https://science.nasa.gov/earth/</t>
   </si>
   <si>
@@ -74,6 +83,9 @@
     <t>red planet</t>
   </si>
   <si>
+    <t>WD:Q111</t>
+  </si>
+  <si>
     <t>https://science.nasa.gov/mars/</t>
   </si>
   <si>
@@ -188,6 +200,9 @@
     <t>the moon</t>
   </si>
   <si>
+    <t>WD:Q405</t>
+  </si>
+  <si>
     <t>https://science.nasa.gov/moon/</t>
   </si>
   <si>
@@ -207,6 +222,9 @@
   </si>
   <si>
     <t>asteroid belt</t>
+  </si>
+  <si>
+    <t>WD:Q2179</t>
   </si>
   <si>
     <t>asteroid</t>
@@ -639,116 +657,128 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink r:id="rId2" ref="E5"/>
-    <hyperlink r:id="rId3" ref="E6"/>
+    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId2" ref="F5"/>
+    <hyperlink r:id="rId3" ref="F6"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
 </worksheet>
@@ -777,34 +807,37 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -838,41 +871,44 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -910,95 +946,101 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E3"/>
-    <hyperlink r:id="rId2" ref="E4"/>
-    <hyperlink r:id="rId3" ref="E7"/>
+    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink r:id="rId2" ref="F4"/>
+    <hyperlink r:id="rId3" ref="F7"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
 </worksheet>
@@ -1027,23 +1069,29 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1077,51 +1125,54 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2"/>
-    <hyperlink r:id="rId2" ref="D3"/>
-    <hyperlink r:id="rId3" ref="D4"/>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId3" ref="E4"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
 </worksheet>
@@ -1153,49 +1204,52 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>70</v>
+        <v>88</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2"/>
-    <hyperlink r:id="rId2" ref="D5"/>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId2" ref="E5"/>
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -1227,141 +1281,144 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>